<commit_message>
updated field counts, etc.  Ready for grading.
</commit_message>
<xml_diff>
--- a/CS5200 Project Rubric.xlsx
+++ b/CS5200 Project Rubric.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doyle\Documents\GitHub\CS5200_MyTinerary\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Category</t>
   </si>
@@ -162,10 +157,25 @@
     <t>Yelp, FlightAware, Facebook</t>
   </si>
   <si>
-    <t>(Auth initial = fb login, but not "real" after that)</t>
-  </si>
-  <si>
-    <t>(most DAO methods are hooked up, but only one used, so only counting that one)</t>
+    <t>2 enums done via JPA, which doesn't create a table</t>
+  </si>
+  <si>
+    <t>bootstrap theme and bootstrap</t>
+  </si>
+  <si>
+    <t>(included jquery and jquery ui, but barely used - I started with javascript and retreated to jsp )as a plan B</t>
+  </si>
+  <si>
+    <t>(Note: Auth initial = fb login, but not "real" after that, so maybe that one doesn't count as much)</t>
+  </si>
+  <si>
+    <t>(most DAO CRUD methods are hooked up, but only one used in UI, so only counting that one)</t>
+  </si>
+  <si>
+    <t>verifyAuthenticatedUser</t>
+  </si>
+  <si>
+    <t>Server side makes calls to Yelp and FlightAware in java, not Ajax.  UI does one ajax call to server "verify" method</t>
   </si>
 </sst>
 </file>
@@ -495,7 +505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -505,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -543,31 +553,44 @@
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -592,7 +615,9 @@
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -606,37 +631,49 @@
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -654,7 +691,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -664,6 +701,9 @@
       <c r="B21" s="4">
         <v>1</v>
       </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
@@ -680,6 +720,9 @@
       <c r="B23" s="4">
         <v>1</v>
       </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
@@ -727,14 +770,16 @@
         <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
@@ -743,26 +788,35 @@
       <c r="B31" s="4">
         <v>1</v>
       </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -770,7 +824,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>36</v>
       </c>
@@ -778,25 +832,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="4"/>
-    </row>
-    <row r="38" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B37" s="4">
+        <f>22+6</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="4"/>
-    </row>
-    <row r="39" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B38" s="4">
+        <f>4+8</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B39" s="4">
+        <f>1+1+4</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>40</v>
       </c>
@@ -804,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>41</v>
       </c>
@@ -812,19 +875,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="4"/>
-    </row>
-    <row r="43" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B42" s="4">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="4"/>
-    </row>
-    <row r="44" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B43" s="4">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>44</v>
       </c>

</xml_diff>